<commit_message>
Ejercicios resueltos antes del examen
</commit_message>
<xml_diff>
--- a/Tarea5/ISR.xlsx
+++ b/Tarea5/ISR.xlsx
@@ -1,31 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hca\Documents\AlgoritmosNum\Tarea5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Documents/AlgoritmosNum/Tarea5/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6572D06E-3EB7-A04D-BA15-FAA14B35E567}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Hoja1!$B$21:$B$31</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Hoja1!$G$20</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Hoja1!$G$21:$G$31</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Hoja1!$B$21:$B$31</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Hoja1!$G$20</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Hoja1!$G$21:$G$31</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Hoja1!$B$21:$B$31</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Hoja1!$G$20</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Hoja1!$G$21:$G$31</definedName>
-  </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -76,7 +66,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
@@ -220,7 +210,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -580,7 +569,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2054,7 +2042,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2084,7 +2078,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Gráfico 3"/>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2364,22 +2364,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S50" sqref="S50"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="68" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="10">
         <v>1</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>1.9199999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
         <v>578.53</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="5">
         <v>4910.1899999999996</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>0.10879999999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="5">
         <v>8629.2099999999991</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
         <v>10031.08</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>0.1792</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
         <v>12009.95</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>0.21360000000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
         <v>24222.32</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>0.23519999999999999</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
         <v>38177.699999999997</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
         <v>72887.509999999995</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="5">
         <v>97183.34</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="5">
         <v>291550.01</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>5</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="6">
         <v>15000</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>13089.455320000001</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="6">
         <v>17429.482044760935</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -2651,326 +2651,326 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="10">
         <v>1</v>
       </c>
       <c r="C21" s="8">
-        <f>LOOKUP($B21,$B$4:$B$14,$B$4:$B$14)</f>
+        <f t="shared" ref="C21:C31" si="0">LOOKUP($B21,$B$4:$B$14,$B$4:$B$14)</f>
         <v>1</v>
       </c>
       <c r="D21" s="8">
-        <f>LOOKUP($B21,$B$4:$B$14,$C$4:$C$14)</f>
+        <f t="shared" ref="D21:D31" si="1">LOOKUP($B21,$B$4:$B$14,$C$4:$C$14)</f>
         <v>578.52</v>
       </c>
       <c r="E21" s="8">
-        <f>LOOKUP($B21,$B$4:$B$14,$D$4:$D$14)</f>
+        <f t="shared" ref="E21:E31" si="2">LOOKUP($B21,$B$4:$B$14,$D$4:$D$14)</f>
         <v>0</v>
       </c>
       <c r="F21" s="7">
-        <f>LOOKUP($B21,$B$4:$B$14,$E$4:$E$14)</f>
+        <f t="shared" ref="F21:F31" si="3">LOOKUP($B21,$B$4:$B$14,$E$4:$E$14)</f>
         <v>1.9199999999999998E-2</v>
       </c>
       <c r="G21" s="9">
-        <f>E21+F21*(B21-C21)</f>
+        <f t="shared" ref="G21:G31" si="4">E21+F21*(B21-C21)</f>
         <v>0</v>
       </c>
       <c r="H21" s="9">
-        <f>B21-G21</f>
+        <f t="shared" ref="H21:H31" si="5">B21-G21</f>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="5">
         <v>578.53</v>
       </c>
       <c r="C22" s="8">
-        <f>LOOKUP($B22,$B$4:$B$14,$B$4:$B$14)</f>
+        <f t="shared" si="0"/>
         <v>578.53</v>
       </c>
       <c r="D22" s="8">
-        <f>LOOKUP($B22,$B$4:$B$14,$C$4:$C$14)</f>
+        <f t="shared" si="1"/>
         <v>4910.18</v>
       </c>
       <c r="E22" s="8">
-        <f>LOOKUP($B22,$B$4:$B$14,$D$4:$D$14)</f>
+        <f t="shared" si="2"/>
         <v>11.11</v>
       </c>
       <c r="F22" s="7">
-        <f>LOOKUP($B22,$B$4:$B$14,$E$4:$E$14)</f>
+        <f t="shared" si="3"/>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="G22" s="9">
-        <f>E22+F22*(B22-C22)</f>
+        <f t="shared" si="4"/>
         <v>11.11</v>
       </c>
       <c r="H22" s="9">
-        <f>B22-G22</f>
+        <f t="shared" si="5"/>
         <v>567.41999999999996</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="5">
         <v>4910.1899999999996</v>
       </c>
       <c r="C23" s="8">
-        <f>LOOKUP($B23,$B$4:$B$14,$B$4:$B$14)</f>
+        <f t="shared" si="0"/>
         <v>4910.1899999999996</v>
       </c>
       <c r="D23" s="8">
-        <f>LOOKUP($B23,$B$4:$B$14,$C$4:$C$14)</f>
+        <f t="shared" si="1"/>
         <v>8629.2000000000007</v>
       </c>
       <c r="E23" s="8">
-        <f>LOOKUP($B23,$B$4:$B$14,$D$4:$D$14)</f>
+        <f t="shared" si="2"/>
         <v>238.33</v>
       </c>
       <c r="F23" s="7">
-        <f>LOOKUP($B23,$B$4:$B$14,$E$4:$E$14)</f>
+        <f t="shared" si="3"/>
         <v>0.10879999999999999</v>
       </c>
       <c r="G23" s="9">
-        <f>E23+F23*(B23-C23)</f>
+        <f t="shared" si="4"/>
         <v>238.33</v>
       </c>
       <c r="H23" s="9">
-        <f>B23-G23</f>
+        <f t="shared" si="5"/>
         <v>4671.8599999999997</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="5">
         <v>8629.2099999999991</v>
       </c>
       <c r="C24" s="8">
-        <f>LOOKUP($B24,$B$4:$B$14,$B$4:$B$14)</f>
+        <f t="shared" si="0"/>
         <v>8629.2099999999991</v>
       </c>
       <c r="D24" s="8">
-        <f>LOOKUP($B24,$B$4:$B$14,$C$4:$C$14)</f>
+        <f t="shared" si="1"/>
         <v>10031.07</v>
       </c>
       <c r="E24" s="8">
-        <f>LOOKUP($B24,$B$4:$B$14,$D$4:$D$14)</f>
+        <f t="shared" si="2"/>
         <v>692.96</v>
       </c>
       <c r="F24" s="7">
-        <f>LOOKUP($B24,$B$4:$B$14,$E$4:$E$14)</f>
+        <f t="shared" si="3"/>
         <v>0.16</v>
       </c>
       <c r="G24" s="9">
-        <f>E24+F24*(B24-C24)</f>
+        <f t="shared" si="4"/>
         <v>692.96</v>
       </c>
       <c r="H24" s="9">
-        <f>B24-G24</f>
+        <f t="shared" si="5"/>
         <v>7936.2499999999991</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="5">
         <v>10031.08</v>
       </c>
       <c r="C25" s="8">
-        <f>LOOKUP($B25,$B$4:$B$14,$B$4:$B$14)</f>
+        <f t="shared" si="0"/>
         <v>10031.08</v>
       </c>
       <c r="D25" s="8">
-        <f>LOOKUP($B25,$B$4:$B$14,$C$4:$C$14)</f>
+        <f t="shared" si="1"/>
         <v>12009.94</v>
       </c>
       <c r="E25" s="8">
-        <f>LOOKUP($B25,$B$4:$B$14,$D$4:$D$14)</f>
+        <f t="shared" si="2"/>
         <v>917.26</v>
       </c>
       <c r="F25" s="7">
-        <f>LOOKUP($B25,$B$4:$B$14,$E$4:$E$14)</f>
+        <f t="shared" si="3"/>
         <v>0.1792</v>
       </c>
       <c r="G25" s="9">
-        <f>E25+F25*(B25-C25)</f>
+        <f t="shared" si="4"/>
         <v>917.26</v>
       </c>
       <c r="H25" s="9">
-        <f>B25-G25</f>
+        <f t="shared" si="5"/>
         <v>9113.82</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="5">
         <v>12009.95</v>
       </c>
       <c r="C26" s="8">
-        <f>LOOKUP($B26,$B$4:$B$14,$B$4:$B$14)</f>
+        <f t="shared" si="0"/>
         <v>12009.95</v>
       </c>
       <c r="D26" s="8">
-        <f>LOOKUP($B26,$B$4:$B$14,$C$4:$C$14)</f>
+        <f t="shared" si="1"/>
         <v>24222.31</v>
       </c>
       <c r="E26" s="8">
-        <f>LOOKUP($B26,$B$4:$B$14,$D$4:$D$14)</f>
+        <f t="shared" si="2"/>
         <v>1271.8699999999999</v>
       </c>
       <c r="F26" s="7">
-        <f>LOOKUP($B26,$B$4:$B$14,$E$4:$E$14)</f>
+        <f t="shared" si="3"/>
         <v>0.21360000000000001</v>
       </c>
       <c r="G26" s="9">
-        <f>E26+F26*(B26-C26)</f>
+        <f t="shared" si="4"/>
         <v>1271.8699999999999</v>
       </c>
       <c r="H26" s="9">
-        <f>B26-G26</f>
+        <f t="shared" si="5"/>
         <v>10738.080000000002</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="5">
         <v>24222.32</v>
       </c>
       <c r="C27" s="8">
-        <f>LOOKUP($B27,$B$4:$B$14,$B$4:$B$14)</f>
+        <f t="shared" si="0"/>
         <v>24222.32</v>
       </c>
       <c r="D27" s="8">
-        <f>LOOKUP($B27,$B$4:$B$14,$C$4:$C$14)</f>
+        <f t="shared" si="1"/>
         <v>38177.69</v>
       </c>
       <c r="E27" s="8">
-        <f>LOOKUP($B27,$B$4:$B$14,$D$4:$D$14)</f>
+        <f t="shared" si="2"/>
         <v>3880.44</v>
       </c>
       <c r="F27" s="7">
-        <f>LOOKUP($B27,$B$4:$B$14,$E$4:$E$14)</f>
+        <f t="shared" si="3"/>
         <v>0.23519999999999999</v>
       </c>
       <c r="G27" s="9">
-        <f>E27+F27*(B27-C27)</f>
+        <f t="shared" si="4"/>
         <v>3880.44</v>
       </c>
       <c r="H27" s="9">
-        <f>B27-G27</f>
+        <f t="shared" si="5"/>
         <v>20341.88</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="5">
         <v>38177.699999999997</v>
       </c>
       <c r="C28" s="8">
-        <f>LOOKUP($B28,$B$4:$B$14,$B$4:$B$14)</f>
+        <f t="shared" si="0"/>
         <v>38177.699999999997</v>
       </c>
       <c r="D28" s="8">
-        <f>LOOKUP($B28,$B$4:$B$14,$C$4:$C$14)</f>
+        <f t="shared" si="1"/>
         <v>72887.5</v>
       </c>
       <c r="E28" s="8">
-        <f>LOOKUP($B28,$B$4:$B$14,$D$4:$D$14)</f>
+        <f t="shared" si="2"/>
         <v>7162.74</v>
       </c>
       <c r="F28" s="7">
-        <f>LOOKUP($B28,$B$4:$B$14,$E$4:$E$14)</f>
+        <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
       <c r="G28" s="9">
-        <f>E28+F28*(B28-C28)</f>
+        <f t="shared" si="4"/>
         <v>7162.74</v>
       </c>
       <c r="H28" s="9">
-        <f>B28-G28</f>
+        <f t="shared" si="5"/>
         <v>31014.959999999999</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" s="5">
         <v>72887.509999999995</v>
       </c>
       <c r="C29" s="8">
-        <f>LOOKUP($B29,$B$4:$B$14,$B$4:$B$14)</f>
+        <f t="shared" si="0"/>
         <v>72887.509999999995</v>
       </c>
       <c r="D29" s="8">
-        <f>LOOKUP($B29,$B$4:$B$14,$C$4:$C$14)</f>
+        <f t="shared" si="1"/>
         <v>97183.33</v>
       </c>
       <c r="E29" s="8">
-        <f>LOOKUP($B29,$B$4:$B$14,$D$4:$D$14)</f>
+        <f t="shared" si="2"/>
         <v>17575.689999999999</v>
       </c>
       <c r="F29" s="7">
-        <f>LOOKUP($B29,$B$4:$B$14,$E$4:$E$14)</f>
+        <f t="shared" si="3"/>
         <v>0.32</v>
       </c>
       <c r="G29" s="9">
-        <f>E29+F29*(B29-C29)</f>
+        <f t="shared" si="4"/>
         <v>17575.689999999999</v>
       </c>
       <c r="H29" s="9">
-        <f>B29-G29</f>
+        <f t="shared" si="5"/>
         <v>55311.819999999992</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="5">
         <v>97183.34</v>
       </c>
       <c r="C30" s="8">
-        <f>LOOKUP($B30,$B$4:$B$14,$B$4:$B$14)</f>
+        <f t="shared" si="0"/>
         <v>97183.34</v>
       </c>
       <c r="D30" s="8">
-        <f>LOOKUP($B30,$B$4:$B$14,$C$4:$C$14)</f>
+        <f t="shared" si="1"/>
         <v>291550</v>
       </c>
       <c r="E30" s="8">
-        <f>LOOKUP($B30,$B$4:$B$14,$D$4:$D$14)</f>
+        <f t="shared" si="2"/>
         <v>25350.35</v>
       </c>
       <c r="F30" s="7">
-        <f>LOOKUP($B30,$B$4:$B$14,$E$4:$E$14)</f>
+        <f t="shared" si="3"/>
         <v>0.34</v>
       </c>
       <c r="G30" s="9">
-        <f>E30+F30*(B30-C30)</f>
+        <f t="shared" si="4"/>
         <v>25350.35</v>
       </c>
       <c r="H30" s="9">
-        <f>B30-G30</f>
+        <f t="shared" si="5"/>
         <v>71832.989999999991</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="5">
         <v>291550.01</v>
       </c>
       <c r="C31" s="8">
-        <f>LOOKUP($B31,$B$4:$B$14,$B$4:$B$14)</f>
+        <f t="shared" si="0"/>
         <v>291550.01</v>
       </c>
       <c r="D31" s="8" t="str">
-        <f>LOOKUP($B31,$B$4:$B$14,$C$4:$C$14)</f>
+        <f t="shared" si="1"/>
         <v>En Adelante</v>
       </c>
       <c r="E31" s="8">
-        <f>LOOKUP($B31,$B$4:$B$14,$D$4:$D$14)</f>
+        <f t="shared" si="2"/>
         <v>91435.02</v>
       </c>
       <c r="F31" s="7">
-        <f>LOOKUP($B31,$B$4:$B$14,$E$4:$E$14)</f>
+        <f t="shared" si="3"/>
         <v>0.35</v>
       </c>
       <c r="G31" s="9">
-        <f>E31+F31*(B31-C31)</f>
+        <f t="shared" si="4"/>
         <v>91435.02</v>
       </c>
       <c r="H31" s="9">
-        <f>B31-G31</f>
+        <f t="shared" si="5"/>
         <v>200114.99</v>
       </c>
     </row>
-    <row r="50" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="19:19" x14ac:dyDescent="0.2">
       <c r="S50" s="11"/>
     </row>
   </sheetData>

</xml_diff>